<commit_message>
Fix hien thi Muon Tra
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -360,7 +360,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,6 +406,14 @@
         <v>2915000</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2915004</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>